<commit_message>
-Se refactorizo automatizador de extractor de informaciópn para 3 ORM
</commit_message>
<xml_diff>
--- a/GitHub/datos.xlsx
+++ b/GitHub/datos.xlsx
@@ -34,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +42,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,28 +461,80 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>SEQUELIZE</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>11/03/2023</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Existen 5 (62%) elementos de JavaScript y 3 (37%) elementos de TypeScript</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>BOOKSHELF</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>11/03/2023</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Existen 2 (100%) elementos de JavaScript y 0 (0%) elementos de TypeScript</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>PRISMA</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>11/03/2023</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D4" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Existen 4 (57%) elementos de JavaScript y 3 (42%) elementos de TypeScript</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Existen 0 (0%) elementos de JavaScript y 7 (100%) elementos de TypeScript</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>